<commit_message>
second commit of ds algo
</commit_message>
<xml_diff>
--- a/dsalgo/src/test/resources/dsalgoexceldata/ExcelData.xlsx
+++ b/dsalgo/src/test/resources/dsalgoexceldata/ExcelData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F62E83-71E6-4210-89FD-40A93BEEF0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23533296-A471-4F5F-AD38-96DF497A5A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,7 +392,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>